<commit_message>
split functions and adapt example script to have proportion of undefined as well in standard table
</commit_message>
<xml_diff>
--- a/resources/country_hesper_key.xlsx
+++ b/resources/country_hesper_key.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted.sharepoint.com/sites/IMPACTHQ-Accountability&amp;Inclusion/Documents partages/General/12_Accountability to Affected People Specialist/07_Hesper Scale/4. REACH HESPER Pilots/DRC MSNA/R/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://acted-my.sharepoint.com/personal/raphael_bacot_impact-initiatives_org/Documents/git/hespeR/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="305" documentId="11_F25DC773A252ABDACC10488E41DA71445ADE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD7B7DBA-8789-47C0-B729-2EB43ECD3255}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="key" sheetId="1" r:id="rId1"/>
@@ -967,7 +967,7 @@
   <dimension ref="A1:Q29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2588,6 +2588,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="d0fa6634-326e-4532-91a2-52bea7ac9212" xsi:nil="true"/>
@@ -2596,15 +2605,6 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2837,6 +2837,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBECC385-800E-4335-845D-57357BC0A1A7}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D0A760A1-5CE3-40AD-BC35-FFB437F9E8F8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2847,14 +2855,21 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DBECC385-800E-4335-845D-57357BC0A1A7}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821DB61A-69B8-4EFE-ADD0-34D0DB190ED7}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="f4877444-78fa-4cfa-bafc-d6c64fafc061"/>
+    <ds:schemaRef ds:uri="d0fa6634-326e-4532-91a2-52bea7ac9212"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{821DB61A-69B8-4EFE-ADD0-34D0DB190ED7}"/>
 </file>
</xml_diff>